<commit_message>
0.0.03 - Finish Members
</commit_message>
<xml_diff>
--- a/Source/Excel/Frame_01.xlsx
+++ b/Source/Excel/Frame_01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>GOST 26020</t>
   </si>
@@ -35,9 +35,6 @@
     <t>000000</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>30SH1</t>
   </si>
   <si>
@@ -99,6 +96,30 @@
   </si>
   <si>
     <t>sectionType</t>
+  </si>
+  <si>
+    <t>isDivided</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>Brace 1</t>
+  </si>
+  <si>
+    <t>Brace 2</t>
   </si>
 </sst>
 </file>
@@ -173,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -207,6 +228,9 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,84 +512,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="8" style="1" customWidth="1"/>
     <col min="3" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="9.140625" style="4"/>
     <col min="6" max="6" width="11.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" style="4" customWidth="1"/>
     <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="4"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="9.7109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="4"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>3</v>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="L1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="B2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="7"/>
+        <v>13</v>
+      </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="7"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="8"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>1</v>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -588,22 +616,25 @@
       <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
         <v>3</v>
       </c>
-      <c r="L3" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>2</v>
+      <c r="M3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -626,222 +657,237 @@
       <c r="H4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
+      <c r="I4" s="6">
+        <v>1</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
       </c>
       <c r="L4" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>4</v>
       </c>
       <c r="H5" s="1">
         <v>90</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="1">
-        <v>5</v>
+      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L5" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>3</v>
+      </c>
+      <c r="M8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>5</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="1">
-        <v>5</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="1">
+        <v>5</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
         <v>3</v>
       </c>
-      <c r="L8" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="1">
-        <v>5</v>
-      </c>
-      <c r="K10" s="1">
-        <v>0</v>
-      </c>
-      <c r="L10" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
-        <v>3</v>
-      </c>
-      <c r="L11" s="1">
+      <c r="M11" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0.0.06 - Start DivideByExistingNodes
</commit_message>
<xml_diff>
--- a/Source/Excel/Frame_01.xlsx
+++ b/Source/Excel/Frame_01.xlsx
@@ -515,7 +515,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>7</v>
@@ -861,7 +861,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
0.0.08 - FINISH DivideMember
</commit_message>
<xml_diff>
--- a/Source/Excel/Frame_01.xlsx
+++ b/Source/Excel/Frame_01.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>GOST 26020</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>Brace 2</t>
+  </si>
+  <si>
+    <t>000010</t>
+  </si>
+  <si>
+    <t>000001</t>
+  </si>
+  <si>
+    <t>B1</t>
   </si>
 </sst>
 </file>
@@ -515,7 +524,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,6 +732,9 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>
@@ -745,10 +757,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="K7" s="1">
         <v>5</v>
@@ -789,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
@@ -841,7 +853,7 @@
         <v>8</v>
       </c>
       <c r="K10" s="1">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="L10" s="1">
         <v>0</v>
@@ -885,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="1">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="M11" s="1">
         <v>5</v>

</xml_diff>

<commit_message>
0.0.09 - FINISH Constraints
</commit_message>
<xml_diff>
--- a/Source/Excel/Frame_01.xlsx
+++ b/Source/Excel/Frame_01.xlsx
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>32</v>
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
0.1.01 - FINISH First part of program
</commit_message>
<xml_diff>
--- a/Source/Excel/Frame_01.xlsx
+++ b/Source/Excel/Frame_01.xlsx
@@ -524,7 +524,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>33</v>

</xml_diff>